<commit_message>
Sent a new, no-numbers data set. In the midst of trying to set the y-axis labels to the tas. Line 82 is death to me. Lines 91-96 show I shouldn't be far off--I think my problem is understanding how these keys work in the context of "domain".
</commit_message>
<xml_diff>
--- a/bingo_data.xlsx
+++ b/bingo_data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="19155" windowHeight="10545"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="19155" windowHeight="10545" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="bingo_data" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="51">
   <si>
     <t>names</t>
   </si>
@@ -134,13 +135,46 @@
   </si>
   <si>
     <t>Vrexigen</t>
+  </si>
+  <si>
+    <t>strat_buckets</t>
+  </si>
+  <si>
+    <t>CNS</t>
+  </si>
+  <si>
+    <t>Phase 2</t>
+  </si>
+  <si>
+    <t>Endocrine Disorder</t>
+  </si>
+  <si>
+    <t>NDA</t>
+  </si>
+  <si>
+    <t>Phase 3</t>
+  </si>
+  <si>
+    <t>Immunology</t>
+  </si>
+  <si>
+    <t>Phase 1</t>
+  </si>
+  <si>
+    <t>Dermatology</t>
+  </si>
+  <si>
+    <t>Ophthalmology</t>
+  </si>
+  <si>
+    <t>Preclinical</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -667,6 +701,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -745,6 +784,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -779,6 +819,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -954,19 +995,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -983,7 +1024,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1004,7 +1045,7 @@
         <v>68.821047717976512</v>
       </c>
       <c r="G2">
-        <f>(F2-$I$2)/($I$3-$I$2)*90+10</f>
+        <f t="shared" ref="G2:G33" si="0">(F2-$I$2)/($I$3-$I$2)*90+10</f>
         <v>100</v>
       </c>
       <c r="H2">
@@ -1019,7 +1060,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1036,11 +1077,11 @@
         <v>6</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F33" si="0">SQRT(D3)</f>
+        <f t="shared" ref="F3:F33" si="1">SQRT(D3)</f>
         <v>45.459664099066991</v>
       </c>
       <c r="G3">
-        <f>(F3-$I$2)/($I$3-$I$2)*90+10</f>
+        <f t="shared" si="0"/>
         <v>68.612676463863991</v>
       </c>
       <c r="H3">
@@ -1055,7 +1096,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1072,15 +1113,15 @@
         <v>6</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41.165476664311811</v>
       </c>
       <c r="G4">
-        <f>(F4-$I$2)/($I$3-$I$2)*90+10</f>
+        <f t="shared" si="0"/>
         <v>62.843195831288249</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1097,15 +1138,15 @@
         <v>10</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35.53275472011704</v>
       </c>
       <c r="G5">
-        <f>(F5-$I$2)/($I$3-$I$2)*90+10</f>
+        <f t="shared" si="0"/>
         <v>55.275319333235736</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1122,15 +1163,15 @@
         <v>6</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35.212904395973929</v>
       </c>
       <c r="G6">
-        <f>(F6-$I$2)/($I$3-$I$2)*90+10</f>
+        <f t="shared" si="0"/>
         <v>54.845582560329376</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1147,15 +1188,15 @@
         <v>6</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32.865377435836635</v>
       </c>
       <c r="G7">
-        <f>(F7-$I$2)/($I$3-$I$2)*90+10</f>
+        <f t="shared" si="0"/>
         <v>51.691548988962062</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1172,15 +1213,15 @@
         <v>10</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32.358426058756322</v>
       </c>
       <c r="G8">
-        <f>(F8-$I$2)/($I$3-$I$2)*90+10</f>
+        <f t="shared" si="0"/>
         <v>51.010431502554717</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1197,15 +1238,15 @@
         <v>6</v>
       </c>
       <c r="F9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32.144836754912909</v>
       </c>
       <c r="G9">
-        <f>(F9-$I$2)/($I$3-$I$2)*90+10</f>
+        <f t="shared" si="0"/>
         <v>50.723462344693502</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1222,15 +1263,15 @@
         <v>6</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32.007765385918461</v>
       </c>
       <c r="G10">
-        <f>(F10-$I$2)/($I$3-$I$2)*90+10</f>
+        <f t="shared" si="0"/>
         <v>50.539299305536552</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1247,15 +1288,15 @@
         <v>6</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>31.766045536075151</v>
       </c>
       <c r="G11">
-        <f>(F11-$I$2)/($I$3-$I$2)*90+10</f>
+        <f t="shared" si="0"/>
         <v>50.214535188140822</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1272,15 +1313,15 @@
         <v>6</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30.166802528607501</v>
       </c>
       <c r="G12">
-        <f>(F12-$I$2)/($I$3-$I$2)*90+10</f>
+        <f t="shared" si="0"/>
         <v>48.065862895988573</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1297,15 +1338,15 @@
         <v>6</v>
       </c>
       <c r="F13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30.040090923630707</v>
       </c>
       <c r="G13">
-        <f>(F13-$I$2)/($I$3-$I$2)*90+10</f>
+        <f t="shared" si="0"/>
         <v>47.895618778342623</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1322,15 +1363,15 @@
         <v>6</v>
       </c>
       <c r="F14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29.476011916472011</v>
       </c>
       <c r="G14">
-        <f>(F14-$I$2)/($I$3-$I$2)*90+10</f>
+        <f t="shared" si="0"/>
         <v>47.137747130564819</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1347,15 +1388,15 @@
         <v>6</v>
       </c>
       <c r="F15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26.875140937304867</v>
       </c>
       <c r="G15">
-        <f>(F15-$I$2)/($I$3-$I$2)*90+10</f>
+        <f t="shared" si="0"/>
         <v>43.643331721334171</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1372,15 +1413,15 @@
         <v>6</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26.246149302326234</v>
       </c>
       <c r="G16">
-        <f>(F16-$I$2)/($I$3-$I$2)*90+10</f>
+        <f t="shared" si="0"/>
         <v>42.798246332957717</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -1397,15 +1438,15 @@
         <v>10</v>
       </c>
       <c r="F17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25.14704364731568</v>
       </c>
       <c r="G17">
-        <f>(F17-$I$2)/($I$3-$I$2)*90+10</f>
+        <f t="shared" si="0"/>
         <v>41.321536504594249</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1422,15 +1463,15 @@
         <v>6</v>
       </c>
       <c r="F18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24.35550920633769</v>
       </c>
       <c r="G18">
-        <f>(F18-$I$2)/($I$3-$I$2)*90+10</f>
+        <f t="shared" si="0"/>
         <v>40.258065778962191</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1447,15 +1488,15 @@
         <v>25</v>
       </c>
       <c r="F19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22.984153919602957</v>
       </c>
       <c r="G19">
-        <f>(F19-$I$2)/($I$3-$I$2)*90+10</f>
+        <f t="shared" si="0"/>
         <v>38.415573366274231</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1472,15 +1513,15 @@
         <v>6</v>
       </c>
       <c r="F20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22.833847684961025</v>
       </c>
       <c r="G20">
-        <f>(F20-$I$2)/($I$3-$I$2)*90+10</f>
+        <f t="shared" si="0"/>
         <v>38.213628546003136</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1497,15 +1538,15 @@
         <v>25</v>
       </c>
       <c r="F21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19.399394516324474</v>
       </c>
       <c r="G21">
-        <f>(F21-$I$2)/($I$3-$I$2)*90+10</f>
+        <f t="shared" si="0"/>
         <v>33.599248912835897</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1522,15 +1563,15 @@
         <v>10</v>
       </c>
       <c r="F22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19.010491613843129</v>
       </c>
       <c r="G22">
-        <f>(F22-$I$2)/($I$3-$I$2)*90+10</f>
+        <f t="shared" si="0"/>
         <v>33.076736144609114</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1547,15 +1588,15 @@
         <v>10</v>
       </c>
       <c r="F23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18.931870523009607</v>
       </c>
       <c r="G23">
-        <f>(F23-$I$2)/($I$3-$I$2)*90+10</f>
+        <f t="shared" si="0"/>
         <v>32.971104318386352</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -1572,15 +1613,15 @@
         <v>6</v>
       </c>
       <c r="F24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18.791937981485571</v>
       </c>
       <c r="G24">
-        <f>(F24-$I$2)/($I$3-$I$2)*90+10</f>
+        <f t="shared" si="0"/>
         <v>32.783097134150339</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1597,15 +1638,15 @@
         <v>6</v>
       </c>
       <c r="F25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18.721097238142853</v>
       </c>
       <c r="G25">
-        <f>(F25-$I$2)/($I$3-$I$2)*90+10</f>
+        <f t="shared" si="0"/>
         <v>32.687918639284199</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1622,15 +1663,15 @@
         <v>10</v>
       </c>
       <c r="F26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18.433667169068666</v>
       </c>
       <c r="G26">
-        <f>(F26-$I$2)/($I$3-$I$2)*90+10</f>
+        <f t="shared" si="0"/>
         <v>32.301740289610464</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -1647,15 +1688,15 @@
         <v>6</v>
       </c>
       <c r="F27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.619509181586189</v>
       </c>
       <c r="G27">
-        <f>(F27-$I$2)/($I$3-$I$2)*90+10</f>
+        <f t="shared" si="0"/>
         <v>31.207873565810878</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -1672,15 +1713,15 @@
         <v>6</v>
       </c>
       <c r="F28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16.395480813321701</v>
       </c>
       <c r="G28">
-        <f>(F28-$I$2)/($I$3-$I$2)*90+10</f>
+        <f t="shared" si="0"/>
         <v>29.56332309573391</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -1697,15 +1738,15 @@
         <v>25</v>
       </c>
       <c r="F29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16.395480813321701</v>
       </c>
       <c r="G29">
-        <f>(F29-$I$2)/($I$3-$I$2)*90+10</f>
+        <f t="shared" si="0"/>
         <v>29.56332309573391</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -1722,15 +1763,15 @@
         <v>6</v>
       </c>
       <c r="F30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16.361374847487603</v>
       </c>
       <c r="G30">
-        <f>(F30-$I$2)/($I$3-$I$2)*90+10</f>
+        <f t="shared" si="0"/>
         <v>29.517499825947752</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -1747,15 +1788,15 @@
         <v>6</v>
       </c>
       <c r="F31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.123007665927808</v>
       </c>
       <c r="G31">
-        <f>(F31-$I$2)/($I$3-$I$2)*90+10</f>
+        <f t="shared" si="0"/>
         <v>25.166572667072273</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -1772,15 +1813,15 @@
         <v>25</v>
       </c>
       <c r="F32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.8346248940859817</v>
       </c>
       <c r="G32">
-        <f>(F32-$I$2)/($I$3-$I$2)*90+10</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -1797,12 +1838,593 @@
         <v>25</v>
       </c>
       <c r="F33" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
       <c r="G33" t="e">
-        <f>(F33-$I$2)/($I$3-$I$2)*90+10</f>
+        <f t="shared" si="0"/>
         <v>#NUM!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <v>521.38460008279401</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>339.80008531156</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>4736.3366093109398</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>902.40706268766996</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>2066.5810595900998</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7">
+        <v>376.33650758342998</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>1080.1330338124001</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9">
+        <v>268.81179113102002</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10">
+        <v>358.41572150803</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <v>722.27320043144005</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12">
+        <v>1009.0816485826</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13">
+        <v>688.86035319668997</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14">
+        <v>1033.2905297950001</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15">
+        <v>268.81179113102002</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16">
+        <v>632.37380423456</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17">
+        <v>910.03597482091004</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18">
+        <v>267.69458691622998</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19">
+        <v>1047.067736859</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20">
+        <v>528.27133141034903</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21">
+        <v>868.83527846218999</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22">
+        <v>310.44710384782002</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23">
+        <v>361.39879135992999</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24">
+        <v>1262.57665840502</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25">
+        <v>1024.4970446458001</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26">
+        <v>1694.5964688639001</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27">
+        <v>350.47948177681002</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" t="s">
+        <v>47</v>
+      </c>
+      <c r="E28" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28">
+        <v>-8.8100542525283903</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29">
+        <v>353.13693313909999</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F30">
+        <v>593.19082873280001</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" t="s">
+        <v>6</v>
+      </c>
+      <c r="F31">
+        <v>1239.948635754</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32">
+        <v>3.3658485017044999</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" t="s">
+        <v>45</v>
+      </c>
+      <c r="E33" t="s">
+        <v>6</v>
+      </c>
+      <c r="F33">
+        <v>172.21333019276</v>
       </c>
     </row>
   </sheetData>

</xml_diff>